<commit_message>
User Type API added
</commit_message>
<xml_diff>
--- a/Documents/ER-Daigram.xlsx
+++ b/Documents/ER-Daigram.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118F81CE-E12F-0541-9350-7EC06BC39ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561AA1BF-3C24-D142-8070-FF2C26D0040F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" activeTab="4" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" activeTab="1" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
   </bookViews>
   <sheets>
     <sheet name="ER-Daigram" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="122">
   <si>
     <t>M_CTL_CONFIG</t>
   </si>
@@ -394,9 +394,6 @@
     <t>M_ACCOUNT_TYPE</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>VARCHAR(200) NOT NULL</t>
   </si>
   <si>
@@ -407,6 +404,9 @@
   </si>
   <si>
     <t>status id</t>
+  </si>
+  <si>
+    <t>DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -3343,8 +3343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7D17F3-EDCF-734A-BF3E-5D3D430502FC}">
   <dimension ref="A3:D45"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3883,10 +3883,10 @@
         <v>35</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>118</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>80</v>
@@ -3898,13 +3898,13 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -3912,9 +3912,15 @@
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
+      <c r="B40" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
@@ -4214,7 +4220,7 @@
   <dimension ref="A2:AG20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4284,7 +4290,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f>Columns!B38</f>
-        <v>Name</v>
+        <v>NAME</v>
       </c>
       <c r="C6" s="3" t="str">
         <f>Columns!C38</f>
@@ -4295,8 +4301,8 @@
         <v>name</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ref="F6:F11" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
-        <v>"Name" VARCHAR(200) NOT NULL,</v>
+        <f t="shared" ref="F6:F9" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
+        <v>"NAME" VARCHAR(200) NOT NULL,</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.2">
@@ -4473,8 +4479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD591B-EA50-FE4F-A794-48E803E9E6A3}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4490,7 +4496,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -4555,7 +4561,7 @@
         <v>status</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ref="F6:F11" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
+        <f t="shared" ref="F6:F7" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
         <v>"STATUS" VARCHAR(20),</v>
       </c>
     </row>
@@ -5649,7 +5655,7 @@
   <dimension ref="A2:AG24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Notification services and file upload service skeleton
</commit_message>
<xml_diff>
--- a/Documents/ER-Daigram.xlsx
+++ b/Documents/ER-Daigram.xlsx
@@ -8,28 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561AA1BF-3C24-D142-8070-FF2C26D0040F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4F683E-ED86-3A46-82B5-659B9C875C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" activeTab="1" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" activeTab="3" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
   </bookViews>
   <sheets>
     <sheet name="ER-Daigram" sheetId="5" r:id="rId1"/>
     <sheet name="Columns" sheetId="7" r:id="rId2"/>
     <sheet name="CommonColumns" sheetId="8" r:id="rId3"/>
-    <sheet name="M_ACCOUNT_TYPE" sheetId="21" r:id="rId4"/>
-    <sheet name="M_STATUS" sheetId="22" r:id="rId5"/>
-    <sheet name="M_SERVICES" sheetId="19" r:id="rId6"/>
-    <sheet name="T_POST" sheetId="18" r:id="rId7"/>
-    <sheet name="T_POST_REQUEST" sheetId="20" r:id="rId8"/>
-    <sheet name="M_CTL_CONFIG" sheetId="6" r:id="rId9"/>
-    <sheet name="M_USER" sheetId="9" r:id="rId10"/>
-    <sheet name="M_USER_ADDRESS" sheetId="10" r:id="rId11"/>
-    <sheet name="T_LOGIN_HIST" sheetId="12" r:id="rId12"/>
-    <sheet name="T_ACTIVITY_HIST" sheetId="13" r:id="rId13"/>
-    <sheet name="M_VEHICLE_TYPE" sheetId="14" r:id="rId14"/>
-    <sheet name="T_USER_VEHICLE" sheetId="15" r:id="rId15"/>
-    <sheet name="M_POLICY" sheetId="17" r:id="rId16"/>
-    <sheet name="T_POLICY_STATUS" sheetId="16" r:id="rId17"/>
+    <sheet name="T_USER_OTP_HIST" sheetId="24" r:id="rId4"/>
+    <sheet name="T_USER_PASSWORD_HIST" sheetId="23" r:id="rId5"/>
+    <sheet name="M_ACCOUNT_TYPE" sheetId="21" r:id="rId6"/>
+    <sheet name="M_STATUS" sheetId="22" r:id="rId7"/>
+    <sheet name="M_SERVICES" sheetId="19" r:id="rId8"/>
+    <sheet name="T_POST" sheetId="18" r:id="rId9"/>
+    <sheet name="T_POST_REQUEST" sheetId="20" r:id="rId10"/>
+    <sheet name="M_CTL_CONFIG" sheetId="6" r:id="rId11"/>
+    <sheet name="M_USER" sheetId="9" r:id="rId12"/>
+    <sheet name="M_USER_ADDRESS" sheetId="10" r:id="rId13"/>
+    <sheet name="T_LOGIN_HIST" sheetId="12" r:id="rId14"/>
+    <sheet name="T_ACTIVITY_HIST" sheetId="13" r:id="rId15"/>
+    <sheet name="M_VEHICLE_TYPE" sheetId="14" r:id="rId16"/>
+    <sheet name="T_USER_VEHICLE" sheetId="15" r:id="rId17"/>
+    <sheet name="M_POLICY" sheetId="17" r:id="rId18"/>
+    <sheet name="T_POLICY_STATUS" sheetId="16" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="127">
   <si>
     <t>M_CTL_CONFIG</t>
   </si>
@@ -193,9 +195,6 @@
     <t>LAST_NAME</t>
   </si>
   <si>
-    <t>PASSWSORD</t>
-  </si>
-  <si>
     <t>VARCHAR(15) NOT NULL</t>
   </si>
   <si>
@@ -407,6 +406,24 @@
   </si>
   <si>
     <t>DESCRIPTION</t>
+  </si>
+  <si>
+    <t>T_USER_PASSWORD_HIST</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>OTP</t>
+  </si>
+  <si>
+    <t>otp</t>
+  </si>
+  <si>
+    <t>VARCHAR(6) NOT NULL</t>
+  </si>
+  <si>
+    <t>T_USER_OTP_HIST</t>
   </si>
 </sst>
 </file>
@@ -824,6 +841,637 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC304FC8-D1FD-F849-A494-A6A7BF905ED8}">
+  <dimension ref="A2:AG14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT("CREATE TABLE ",CHAR(34),B2,CHAR(34),"(")</f>
+        <v>CREATE TABLE "T_POST_REQUEST"(</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f>Columns!B10</f>
+        <v>ID</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <f>Columns!C10</f>
+        <v>VARCHAR(50) NOT NULL</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>Columns!D10</f>
+        <v>table id</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT(CHAR(34),B5, CHAR(34)," ",C5, ",")</f>
+        <v>"ID" VARCHAR(50) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f>A5+1</f>
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <f>Columns!B37</f>
+        <v>POST_ID</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f>Columns!C37</f>
+        <v>VARCHAR(50) NOT NULL</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>Columns!D37</f>
+        <v>Post table id</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F13" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
+        <v>"POST_ID" VARCHAR(50) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" ref="A7:A14" si="1">A6+1</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="str">
+        <f>Columns!B36</f>
+        <v>REQUEST_USER_ID</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f>Columns!C36</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>Columns!D36</f>
+        <v>User Id</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>"REQUEST_USER_ID" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="str">
+        <f>Columns!B23</f>
+        <v>STATUS</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>Columns!D23</f>
+        <v>status</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>"STATUS" VARCHAR(50) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f>CommonColumns!B4</f>
+        <v>DEL_FLG</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f>CommonColumns!C4</f>
+        <v>int DEFAULT 0</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>CommonColumns!D4</f>
+        <v>delete flag</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>"DEL_FLG" int DEFAULT 0,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="str">
+        <f>CommonColumns!B5</f>
+        <v>INS_DT</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f>CommonColumns!C5</f>
+        <v>TIMESTAMP DEFAULT CURRENT_TIMESTAMP</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f>CommonColumns!D5</f>
+        <v>Inserted date</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_DT" TIMESTAMP DEFAULT CURRENT_TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f>CommonColumns!B6</f>
+        <v>INS_BY</v>
+      </c>
+      <c r="C11" s="3" t="str">
+        <f>CommonColumns!C6</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f>CommonColumns!D6</f>
+        <v xml:space="preserve">Inserted by </v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_BY" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f>CommonColumns!B7</f>
+        <v>UPD_DT</v>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f>CommonColumns!C7</f>
+        <v>TIMESTAMP</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>CommonColumns!D7</f>
+        <v>Updated date</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>"UPD_DT" TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f>CommonColumns!B8</f>
+        <v>UPD_BY</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f>CommonColumns!C8</f>
+        <v>VARCHAR(250)</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f>CommonColumns!D8</f>
+        <v>Updated by</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>"UPD_BY" VARCHAR(250),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AD811D-9B4C-B744-B95C-0E48158B425D}">
+  <dimension ref="A2:AG24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT("CREATE TABLE ",CHAR(34),B2,CHAR(34),"(")</f>
+        <v>CREATE TABLE "M_CTL_CONFIG"(</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f>Columns!B4</f>
+        <v>CTL_CD</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <f>Columns!C4</f>
+        <v>VARCHAR(20) NOT NULL</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>Columns!D4</f>
+        <v>Control code/Service code</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT(CHAR(34),B5, CHAR(34)," ",C5, ",")</f>
+        <v>"CTL_CD" VARCHAR(20) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f>A5+1</f>
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <f>Columns!B5</f>
+        <v>CTL_TYP</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f>Columns!C5</f>
+        <v>VARCHAR(20) NOT NULL</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>Columns!D5</f>
+        <v>Cntrol Type</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F15" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
+        <v>"CTL_TYP" VARCHAR(20) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" ref="A7:A24" si="1">A6+1</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="str">
+        <f>Columns!B6</f>
+        <v>CTL_NO</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f>Columns!C6</f>
+        <v>int NOT NULL</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>Columns!D6</f>
+        <v>Cntrol number</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>"CTL_NO" int NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="str">
+        <f>Columns!B7</f>
+        <v>CTL_DESC</v>
+      </c>
+      <c r="C8" s="3" t="str">
+        <f>Columns!C7</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>Columns!D7</f>
+        <v>Control description</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>"CTL_DESC" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f>Columns!B8</f>
+        <v>CTL_VALUE</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f>Columns!C8</f>
+        <v>TEXT NOT NULL</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>Columns!D8</f>
+        <v>Control value</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>"CTL_VALUE" TEXT NOT NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="str">
+        <f>Columns!B9</f>
+        <v>ON_LOAD</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f>Columns!C9</f>
+        <v>int NOT NULL</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f>Columns!D9</f>
+        <v>on load config flag</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>"ON_LOAD" int NOT NULL,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f>CommonColumns!B4</f>
+        <v>DEL_FLG</v>
+      </c>
+      <c r="C11" s="3" t="str">
+        <f>CommonColumns!C4</f>
+        <v>int DEFAULT 0</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f>CommonColumns!D4</f>
+        <v>delete flag</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>"DEL_FLG" int DEFAULT 0,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f>CommonColumns!B5</f>
+        <v>INS_DT</v>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f>CommonColumns!C5</f>
+        <v>TIMESTAMP DEFAULT CURRENT_TIMESTAMP</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>CommonColumns!D5</f>
+        <v>Inserted date</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_DT" TIMESTAMP DEFAULT CURRENT_TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f>CommonColumns!B6</f>
+        <v>INS_BY</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f>CommonColumns!C6</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f>CommonColumns!D6</f>
+        <v xml:space="preserve">Inserted by </v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_BY" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f>CommonColumns!B7</f>
+        <v>UPD_DT</v>
+      </c>
+      <c r="C14" s="3" t="str">
+        <f>CommonColumns!C7</f>
+        <v>TIMESTAMP</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f>CommonColumns!D7</f>
+        <v>Updated date</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>"UPD_DT" TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="str">
+        <f>CommonColumns!B8</f>
+        <v>UPD_BY</v>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f>CommonColumns!C8</f>
+        <v>VARCHAR(250)</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f>CommonColumns!D8</f>
+        <v>Updated by</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>"UPD_BY" VARCHAR(250),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9B7392-FE9F-F747-B05E-B981C78D453E}">
   <dimension ref="A2:AG24"/>
   <sheetViews>
@@ -844,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -1030,7 +1678,7 @@
       </c>
       <c r="B12" s="3" t="str">
         <f>Columns!B17</f>
-        <v>PASSWSORD</v>
+        <v>PASSWORD</v>
       </c>
       <c r="C12" s="3" t="str">
         <f>Columns!C17</f>
@@ -1042,7 +1690,7 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>"PASSWSORD" VARCHAR(500) NOT NULL,</v>
+        <v>"PASSWORD" VARCHAR(500) NOT NULL,</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.2">
@@ -1242,7 +1890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FE9150-F59C-4A4E-8EB6-891E9048BF8A}">
   <dimension ref="A2:AG21"/>
   <sheetViews>
@@ -1263,7 +1911,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -1553,7 +2201,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384D8DE8-0965-F64B-8C2A-D300CDFFB3FB}">
   <dimension ref="A2:AG21"/>
   <sheetViews>
@@ -1574,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -1842,7 +2490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DBAF1E-4933-134E-A3FD-182B7B61EC8E}">
   <dimension ref="A2:AG21"/>
   <sheetViews>
@@ -1863,7 +2511,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -2148,7 +2796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3904D980-CEDE-5743-8B63-1257231D2A23}">
   <dimension ref="A2:AG21"/>
   <sheetViews>
@@ -2169,7 +2817,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -2456,7 +3104,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0901BE-2902-F441-8B85-BC80ADEE1014}">
   <dimension ref="A2:AG22"/>
   <sheetViews>
@@ -2477,7 +3125,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -2786,7 +3434,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F53C9A-49D3-214D-9338-8DAD7FE9EE51}">
   <dimension ref="A2:AG18"/>
   <sheetViews>
@@ -2807,7 +3455,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -3054,7 +3702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0003AC-73A6-714F-9EC1-A32D17819750}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
@@ -3075,7 +3723,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -3343,8 +3991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7D17F3-EDCF-734A-BF3E-5D3D430502FC}">
   <dimension ref="A3:D45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3484,7 +4132,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3499,7 +4147,7 @@
         <v>25</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3514,7 +4162,7 @@
         <v>26</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3526,10 +4174,10 @@
         <v>47</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3544,7 +4192,7 @@
         <v>26</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3559,7 +4207,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3568,13 +4216,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3583,13 +4231,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3598,13 +4246,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3613,13 +4261,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3628,13 +4276,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3643,13 +4291,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3658,13 +4306,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -3673,13 +4321,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -3688,13 +4336,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3703,13 +4351,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3718,13 +4366,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3733,13 +4381,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -3748,13 +4396,13 @@
         <v>26</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -3763,13 +4411,13 @@
         <v>27</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3778,13 +4426,13 @@
         <v>28</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -3793,13 +4441,13 @@
         <v>29</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -3808,13 +4456,13 @@
         <v>30</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3823,13 +4471,13 @@
         <v>31</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3838,13 +4486,13 @@
         <v>32</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="D35" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3853,13 +4501,13 @@
         <v>33</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -3868,13 +4516,13 @@
         <v>34</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -3883,13 +4531,13 @@
         <v>35</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -3898,13 +4546,13 @@
         <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -3913,10 +4561,10 @@
         <v>37</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>5</v>
@@ -3927,9 +4575,15 @@
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
+      <c r="B41" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
@@ -4216,6 +4870,526 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAD4CD2-793C-F541-AD63-B0A103A94339}">
+  <dimension ref="A2:AG20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT("CREATE TABLE ",CHAR(34),B2,CHAR(34),"(")</f>
+        <v>CREATE TABLE "T_USER_OTP_HIST"(</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f>Columns!B11</f>
+        <v>USER_ID</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <f>Columns!C11</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>Columns!D11</f>
+        <v>User Id</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT(CHAR(34),B5, CHAR(34)," ",C5, ",")</f>
+        <v>"USER_ID" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f>A5+1</f>
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <f>Columns!B12</f>
+        <v>AC_TYP</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f>Columns!C12</f>
+        <v>int NOT NULL</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>Columns!D12</f>
+        <v>Account type</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F9" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
+        <v>"AC_TYP" int NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" ref="A7:A20" si="1">A6+1</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="str">
+        <f>Columns!B41</f>
+        <v>OTP</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f>Columns!C41</f>
+        <v>VARCHAR(6) NOT NULL</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>Columns!D41</f>
+        <v>otp</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>"OTP" VARCHAR(6) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="str">
+        <f>CommonColumns!B5</f>
+        <v>INS_DT</v>
+      </c>
+      <c r="C8" s="3" t="str">
+        <f>CommonColumns!C5</f>
+        <v>TIMESTAMP DEFAULT CURRENT_TIMESTAMP</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>CommonColumns!D5</f>
+        <v>Inserted date</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_DT" TIMESTAMP DEFAULT CURRENT_TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f>CommonColumns!B6</f>
+        <v>INS_BY</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f>CommonColumns!C6</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>CommonColumns!D6</f>
+        <v xml:space="preserve">Inserted by </v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_BY" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705A2A03-52BE-704A-B9B0-E08FD94F4E0C}">
+  <dimension ref="A2:AG20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT("CREATE TABLE ",CHAR(34),B2,CHAR(34),"(")</f>
+        <v>CREATE TABLE "T_USER_PASSWORD_HIST"(</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f>Columns!B11</f>
+        <v>USER_ID</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <f>Columns!C11</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>Columns!D11</f>
+        <v>User Id</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT(CHAR(34),B5, CHAR(34)," ",C5, ",")</f>
+        <v>"USER_ID" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f>A5+1</f>
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <f>Columns!B12</f>
+        <v>AC_TYP</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f>Columns!C12</f>
+        <v>int NOT NULL</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>Columns!D12</f>
+        <v>Account type</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F9" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
+        <v>"AC_TYP" int NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" ref="A7:A20" si="1">A6+1</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="str">
+        <f>Columns!B17</f>
+        <v>PASSWORD</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f>Columns!C17</f>
+        <v>VARCHAR(500) NOT NULL</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>Columns!D17</f>
+        <v>password</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>"PASSWORD" VARCHAR(500) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="str">
+        <f>CommonColumns!B5</f>
+        <v>INS_DT</v>
+      </c>
+      <c r="C8" s="3" t="str">
+        <f>CommonColumns!C5</f>
+        <v>TIMESTAMP DEFAULT CURRENT_TIMESTAMP</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>CommonColumns!D5</f>
+        <v>Inserted date</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_DT" TIMESTAMP DEFAULT CURRENT_TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f>CommonColumns!B6</f>
+        <v>INS_BY</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f>CommonColumns!C6</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>CommonColumns!D6</f>
+        <v xml:space="preserve">Inserted by </v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_BY" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B493808A-68C4-EA4D-94DE-B822277B2CB8}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
@@ -4236,7 +5410,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -4475,7 +5649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD591B-EA50-FE4F-A794-48E803E9E6A3}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
@@ -4496,7 +5670,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -4709,7 +5883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1940831B-3034-354F-A9B0-BA947E4E5A0B}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
@@ -4730,7 +5904,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -4995,7 +6169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D308D1A-EFEE-6845-8598-73802D5A6ADD}">
   <dimension ref="A2:AG21"/>
   <sheetViews>
@@ -5016,7 +6190,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.2">
@@ -5391,635 +6565,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC304FC8-D1FD-F849-A494-A6A7BF905ED8}">
-  <dimension ref="A2:AG14"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="AG3" s="1"/>
-    </row>
-    <row r="4" spans="1:33" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="str">
-        <f>_xlfn.CONCAT("CREATE TABLE ",CHAR(34),B2,CHAR(34),"(")</f>
-        <v>CREATE TABLE "T_POST_REQUEST"(</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="str">
-        <f>Columns!B10</f>
-        <v>ID</v>
-      </c>
-      <c r="C5" s="3" t="str">
-        <f>Columns!C10</f>
-        <v>VARCHAR(50) NOT NULL</v>
-      </c>
-      <c r="D5" s="3" t="str">
-        <f>Columns!D10</f>
-        <v>table id</v>
-      </c>
-      <c r="F5" t="str">
-        <f>_xlfn.CONCAT(CHAR(34),B5, CHAR(34)," ",C5, ",")</f>
-        <v>"ID" VARCHAR(50) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <f>A5+1</f>
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="str">
-        <f>Columns!B37</f>
-        <v>POST_ID</v>
-      </c>
-      <c r="C6" s="3" t="str">
-        <f>Columns!C37</f>
-        <v>VARCHAR(50) NOT NULL</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f>Columns!D37</f>
-        <v>Post table id</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" ref="F6:F13" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
-        <v>"POST_ID" VARCHAR(50) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <f t="shared" ref="A7:A14" si="1">A6+1</f>
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="str">
-        <f>Columns!B36</f>
-        <v>REQUEST_USER_ID</v>
-      </c>
-      <c r="C7" s="3" t="str">
-        <f>Columns!C36</f>
-        <v>VARCHAR(250) NOT NULL</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f>Columns!D36</f>
-        <v>User Id</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>"REQUEST_USER_ID" VARCHAR(250) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="str">
-        <f>Columns!B23</f>
-        <v>STATUS</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f>Columns!D23</f>
-        <v>status</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>"STATUS" VARCHAR(50) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="str">
-        <f>CommonColumns!B4</f>
-        <v>DEL_FLG</v>
-      </c>
-      <c r="C9" s="3" t="str">
-        <f>CommonColumns!C4</f>
-        <v>int DEFAULT 0</v>
-      </c>
-      <c r="D9" s="3" t="str">
-        <f>CommonColumns!D4</f>
-        <v>delete flag</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>"DEL_FLG" int DEFAULT 0,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="str">
-        <f>CommonColumns!B5</f>
-        <v>INS_DT</v>
-      </c>
-      <c r="C10" s="3" t="str">
-        <f>CommonColumns!C5</f>
-        <v>TIMESTAMP DEFAULT CURRENT_TIMESTAMP</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f>CommonColumns!D5</f>
-        <v>Inserted date</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>"INS_DT" TIMESTAMP DEFAULT CURRENT_TIMESTAMP,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="str">
-        <f>CommonColumns!B6</f>
-        <v>INS_BY</v>
-      </c>
-      <c r="C11" s="3" t="str">
-        <f>CommonColumns!C6</f>
-        <v>VARCHAR(250) NOT NULL</v>
-      </c>
-      <c r="D11" s="3" t="str">
-        <f>CommonColumns!D6</f>
-        <v xml:space="preserve">Inserted by </v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>"INS_BY" VARCHAR(250) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="str">
-        <f>CommonColumns!B7</f>
-        <v>UPD_DT</v>
-      </c>
-      <c r="C12" s="3" t="str">
-        <f>CommonColumns!C7</f>
-        <v>TIMESTAMP</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f>CommonColumns!D7</f>
-        <v>Updated date</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>"UPD_DT" TIMESTAMP,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="str">
-        <f>CommonColumns!B8</f>
-        <v>UPD_BY</v>
-      </c>
-      <c r="C13" s="3" t="str">
-        <f>CommonColumns!C8</f>
-        <v>VARCHAR(250)</v>
-      </c>
-      <c r="D13" s="3" t="str">
-        <f>CommonColumns!D8</f>
-        <v>Updated by</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>"UPD_BY" VARCHAR(250),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AD811D-9B4C-B744-B95C-0E48158B425D}">
-  <dimension ref="A2:AG24"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="AG3" s="1"/>
-    </row>
-    <row r="4" spans="1:33" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="str">
-        <f>_xlfn.CONCAT("CREATE TABLE ",CHAR(34),B2,CHAR(34),"(")</f>
-        <v>CREATE TABLE "M_CTL_CONFIG"(</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="str">
-        <f>Columns!B4</f>
-        <v>CTL_CD</v>
-      </c>
-      <c r="C5" s="3" t="str">
-        <f>Columns!C4</f>
-        <v>VARCHAR(20) NOT NULL</v>
-      </c>
-      <c r="D5" s="3" t="str">
-        <f>Columns!D4</f>
-        <v>Control code/Service code</v>
-      </c>
-      <c r="F5" t="str">
-        <f>_xlfn.CONCAT(CHAR(34),B5, CHAR(34)," ",C5, ",")</f>
-        <v>"CTL_CD" VARCHAR(20) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <f>A5+1</f>
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="str">
-        <f>Columns!B5</f>
-        <v>CTL_TYP</v>
-      </c>
-      <c r="C6" s="3" t="str">
-        <f>Columns!C5</f>
-        <v>VARCHAR(20) NOT NULL</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f>Columns!D5</f>
-        <v>Cntrol Type</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" ref="F6:F15" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
-        <v>"CTL_TYP" VARCHAR(20) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <f t="shared" ref="A7:A24" si="1">A6+1</f>
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="str">
-        <f>Columns!B6</f>
-        <v>CTL_NO</v>
-      </c>
-      <c r="C7" s="3" t="str">
-        <f>Columns!C6</f>
-        <v>int NOT NULL</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f>Columns!D6</f>
-        <v>Cntrol number</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>"CTL_NO" int NOT NULL,</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="str">
-        <f>Columns!B7</f>
-        <v>CTL_DESC</v>
-      </c>
-      <c r="C8" s="3" t="str">
-        <f>Columns!C7</f>
-        <v>VARCHAR(250) NOT NULL</v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f>Columns!D7</f>
-        <v>Control description</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>"CTL_DESC" VARCHAR(250) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="str">
-        <f>Columns!B8</f>
-        <v>CTL_VALUE</v>
-      </c>
-      <c r="C9" s="3" t="str">
-        <f>Columns!C8</f>
-        <v>TEXT NOT NULL</v>
-      </c>
-      <c r="D9" s="3" t="str">
-        <f>Columns!D8</f>
-        <v>Control value</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>"CTL_VALUE" TEXT NOT NULL,</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="str">
-        <f>Columns!B9</f>
-        <v>ON_LOAD</v>
-      </c>
-      <c r="C10" s="3" t="str">
-        <f>Columns!C9</f>
-        <v>int NOT NULL</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f>Columns!D9</f>
-        <v>on load config flag</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>"ON_LOAD" int NOT NULL,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="str">
-        <f>CommonColumns!B4</f>
-        <v>DEL_FLG</v>
-      </c>
-      <c r="C11" s="3" t="str">
-        <f>CommonColumns!C4</f>
-        <v>int DEFAULT 0</v>
-      </c>
-      <c r="D11" s="3" t="str">
-        <f>CommonColumns!D4</f>
-        <v>delete flag</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>"DEL_FLG" int DEFAULT 0,</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="str">
-        <f>CommonColumns!B5</f>
-        <v>INS_DT</v>
-      </c>
-      <c r="C12" s="3" t="str">
-        <f>CommonColumns!C5</f>
-        <v>TIMESTAMP DEFAULT CURRENT_TIMESTAMP</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f>CommonColumns!D5</f>
-        <v>Inserted date</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>"INS_DT" TIMESTAMP DEFAULT CURRENT_TIMESTAMP,</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="str">
-        <f>CommonColumns!B6</f>
-        <v>INS_BY</v>
-      </c>
-      <c r="C13" s="3" t="str">
-        <f>CommonColumns!C6</f>
-        <v>VARCHAR(250) NOT NULL</v>
-      </c>
-      <c r="D13" s="3" t="str">
-        <f>CommonColumns!D6</f>
-        <v xml:space="preserve">Inserted by </v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>"INS_BY" VARCHAR(250) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="str">
-        <f>CommonColumns!B7</f>
-        <v>UPD_DT</v>
-      </c>
-      <c r="C14" s="3" t="str">
-        <f>CommonColumns!C7</f>
-        <v>TIMESTAMP</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f>CommonColumns!D7</f>
-        <v>Updated date</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>"UPD_DT" TIMESTAMP,</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B15" s="3" t="str">
-        <f>CommonColumns!B8</f>
-        <v>UPD_BY</v>
-      </c>
-      <c r="C15" s="3" t="str">
-        <f>CommonColumns!C8</f>
-        <v>VARCHAR(250)</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f>CommonColumns!D8</f>
-        <v>Updated by</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>"UPD_BY" VARCHAR(250),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Post Bid create api
</commit_message>
<xml_diff>
--- a/Documents/ER-Daigram.xlsx
+++ b/Documents/ER-Daigram.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev/booking/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rautatul/Documents/Atul/Study/Projects/booking-dev-int/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4F683E-ED86-3A46-82B5-659B9C875C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BAD306-C290-3F4F-8EFD-53D8F57981BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" activeTab="3" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="27640" windowHeight="15800" xr2:uid="{90052BEC-FEBB-F247-ACB1-709744DE85BE}"/>
   </bookViews>
   <sheets>
     <sheet name="ER-Daigram" sheetId="5" r:id="rId1"/>
     <sheet name="Columns" sheetId="7" r:id="rId2"/>
     <sheet name="CommonColumns" sheetId="8" r:id="rId3"/>
-    <sheet name="T_USER_OTP_HIST" sheetId="24" r:id="rId4"/>
-    <sheet name="T_USER_PASSWORD_HIST" sheetId="23" r:id="rId5"/>
-    <sheet name="M_ACCOUNT_TYPE" sheetId="21" r:id="rId6"/>
-    <sheet name="M_STATUS" sheetId="22" r:id="rId7"/>
-    <sheet name="M_SERVICES" sheetId="19" r:id="rId8"/>
-    <sheet name="T_POST" sheetId="18" r:id="rId9"/>
-    <sheet name="T_POST_REQUEST" sheetId="20" r:id="rId10"/>
-    <sheet name="M_CTL_CONFIG" sheetId="6" r:id="rId11"/>
-    <sheet name="M_USER" sheetId="9" r:id="rId12"/>
-    <sheet name="M_USER_ADDRESS" sheetId="10" r:id="rId13"/>
-    <sheet name="T_LOGIN_HIST" sheetId="12" r:id="rId14"/>
-    <sheet name="T_ACTIVITY_HIST" sheetId="13" r:id="rId15"/>
-    <sheet name="M_VEHICLE_TYPE" sheetId="14" r:id="rId16"/>
-    <sheet name="T_USER_VEHICLE" sheetId="15" r:id="rId17"/>
-    <sheet name="M_POLICY" sheetId="17" r:id="rId18"/>
-    <sheet name="T_POLICY_STATUS" sheetId="16" r:id="rId19"/>
+    <sheet name="T_POST_BID" sheetId="25" r:id="rId4"/>
+    <sheet name="T_USER_OTP_HIST" sheetId="24" r:id="rId5"/>
+    <sheet name="T_USER_PASSWORD_HIST" sheetId="23" r:id="rId6"/>
+    <sheet name="M_ACCOUNT_TYPE" sheetId="21" r:id="rId7"/>
+    <sheet name="M_STATUS" sheetId="22" r:id="rId8"/>
+    <sheet name="M_SERVICES" sheetId="19" r:id="rId9"/>
+    <sheet name="T_POST" sheetId="18" r:id="rId10"/>
+    <sheet name="T_POST_REQUEST" sheetId="20" r:id="rId11"/>
+    <sheet name="M_CTL_CONFIG" sheetId="6" r:id="rId12"/>
+    <sheet name="M_USER" sheetId="9" r:id="rId13"/>
+    <sheet name="M_USER_ADDRESS" sheetId="10" r:id="rId14"/>
+    <sheet name="T_LOGIN_HIST" sheetId="12" r:id="rId15"/>
+    <sheet name="T_ACTIVITY_HIST" sheetId="13" r:id="rId16"/>
+    <sheet name="M_VEHICLE_TYPE" sheetId="14" r:id="rId17"/>
+    <sheet name="T_USER_VEHICLE" sheetId="15" r:id="rId18"/>
+    <sheet name="M_POLICY" sheetId="17" r:id="rId19"/>
+    <sheet name="T_POLICY_STATUS" sheetId="16" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="130">
   <si>
     <t>M_CTL_CONFIG</t>
   </si>
@@ -424,6 +425,15 @@
   </si>
   <si>
     <t>T_USER_OTP_HIST</t>
+  </si>
+  <si>
+    <t>T_POST_BID</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -825,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1749B122-D48B-9A47-9252-07DC068BCFB8}">
   <dimension ref="B3:G3"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="AT6" sqref="AT6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -841,6 +851,404 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D308D1A-EFEE-6845-8598-73802D5A6ADD}">
+  <dimension ref="A2:AG21"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT("CREATE TABLE ",CHAR(34),B2,CHAR(34),"(")</f>
+        <v>CREATE TABLE "T_POST"(</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f>Columns!B10</f>
+        <v>ID</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <f>Columns!C10</f>
+        <v>VARCHAR(50) NOT NULL</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>Columns!D10</f>
+        <v>table id</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT(CHAR(34),B5, CHAR(34)," ",C5, ",")</f>
+        <v>"ID" VARCHAR(50) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f>A5+1</f>
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <f>Columns!B11</f>
+        <v>USER_ID</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f>Columns!C11</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>Columns!D11</f>
+        <v>User Id</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F19" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
+        <v>"USER_ID" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" ref="A7:A21" si="1">A6+1</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="str">
+        <f>Columns!B31</f>
+        <v>SERVICE_ID</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f>Columns!C31</f>
+        <v>VARCHAR(50) NOT NULL</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>Columns!D31</f>
+        <v>M_SERVICE table id</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>"SERVICE_ID" VARCHAR(50) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="str">
+        <f>Columns!B25</f>
+        <v>VEHICLE_ID</v>
+      </c>
+      <c r="C8" s="3" t="str">
+        <f>Columns!C25</f>
+        <v xml:space="preserve">VARCHAR(50) </v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>Columns!D25</f>
+        <v>Velicle master table id</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>"VEHICLE_ID" VARCHAR(50) ,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f>Columns!B32</f>
+        <v>ACTIVITY_DATE_TIME_FROM</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f>Columns!C32</f>
+        <v>VARCHAR(25)</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>Columns!D32</f>
+        <v>Activity date time from</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>"ACTIVITY_DATE_TIME_FROM" VARCHAR(25),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="str">
+        <f>Columns!B33</f>
+        <v>ACTIVITY_DATE_TIME_TO</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f>Columns!C33</f>
+        <v>VARCHAR(25)</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f>Columns!D33</f>
+        <v>Activity date time to</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>"ACTIVITY_DATE_TIME_TO" VARCHAR(25),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f>Columns!B34</f>
+        <v>SOURCE</v>
+      </c>
+      <c r="C11" s="3" t="str">
+        <f>Columns!C34</f>
+        <v>VARCHAR(500)</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f>Columns!D34</f>
+        <v>Source adderss</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>"SOURCE" VARCHAR(500),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f>Columns!B35</f>
+        <v>DESTINATION</v>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f>Columns!C35</f>
+        <v>VARCHAR(500)</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>Columns!D35</f>
+        <v>Destination address</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>"DESTINATION" VARCHAR(500),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f>Columns!B22</f>
+        <v>OTHER</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f>Columns!C22</f>
+        <v>TEXT</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f>Columns!D22</f>
+        <v>other details</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>"OTHER" TEXT,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="str">
+        <f>Columns!B23</f>
+        <v>STATUS</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f>Columns!D23</f>
+        <v>status</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>"STATUS" VARCHAR(50) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="str">
+        <f>CommonColumns!B4</f>
+        <v>DEL_FLG</v>
+      </c>
+      <c r="C15" s="3" t="str">
+        <f>CommonColumns!C4</f>
+        <v>int DEFAULT 0</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f>CommonColumns!D4</f>
+        <v>delete flag</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>"DEL_FLG" int DEFAULT 0,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="str">
+        <f>CommonColumns!B5</f>
+        <v>INS_DT</v>
+      </c>
+      <c r="C16" s="3" t="str">
+        <f>CommonColumns!C5</f>
+        <v>TIMESTAMP DEFAULT CURRENT_TIMESTAMP</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f>CommonColumns!D5</f>
+        <v>Inserted date</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_DT" TIMESTAMP DEFAULT CURRENT_TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="str">
+        <f>CommonColumns!B6</f>
+        <v>INS_BY</v>
+      </c>
+      <c r="C17" s="3" t="str">
+        <f>CommonColumns!C6</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f>CommonColumns!D6</f>
+        <v xml:space="preserve">Inserted by </v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_BY" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="str">
+        <f>CommonColumns!B7</f>
+        <v>UPD_DT</v>
+      </c>
+      <c r="C18" s="3" t="str">
+        <f>CommonColumns!C7</f>
+        <v>TIMESTAMP</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f>CommonColumns!D7</f>
+        <v>Updated date</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>"UPD_DT" TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="str">
+        <f>CommonColumns!B8</f>
+        <v>UPD_BY</v>
+      </c>
+      <c r="C19" s="3" t="str">
+        <f>CommonColumns!C8</f>
+        <v>VARCHAR(250)</v>
+      </c>
+      <c r="D19" s="3" t="str">
+        <f>CommonColumns!D8</f>
+        <v>Updated by</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>"UPD_BY" VARCHAR(250),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC304FC8-D1FD-F849-A494-A6A7BF905ED8}">
   <dimension ref="A2:AG14"/>
   <sheetViews>
@@ -1097,7 +1505,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00AD811D-9B4C-B744-B95C-0E48158B425D}">
   <dimension ref="A2:AG24"/>
   <sheetViews>
@@ -1471,7 +1879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C9B7392-FE9F-F747-B05E-B981C78D453E}">
   <dimension ref="A2:AG24"/>
   <sheetViews>
@@ -1890,7 +2298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FE9150-F59C-4A4E-8EB6-891E9048BF8A}">
   <dimension ref="A2:AG21"/>
   <sheetViews>
@@ -2201,7 +2609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384D8DE8-0965-F64B-8C2A-D300CDFFB3FB}">
   <dimension ref="A2:AG21"/>
   <sheetViews>
@@ -2490,7 +2898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DBAF1E-4933-134E-A3FD-182B7B61EC8E}">
   <dimension ref="A2:AG21"/>
   <sheetViews>
@@ -2796,7 +3204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3904D980-CEDE-5743-8B63-1257231D2A23}">
   <dimension ref="A2:AG21"/>
   <sheetViews>
@@ -3104,7 +3512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0901BE-2902-F441-8B85-BC80ADEE1014}">
   <dimension ref="A2:AG22"/>
   <sheetViews>
@@ -3434,7 +3842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F53C9A-49D3-214D-9338-8DAD7FE9EE51}">
   <dimension ref="A2:AG18"/>
   <sheetViews>
@@ -3702,7 +4110,652 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7D17F3-EDCF-734A-BF3E-5D3D430502FC}">
+  <dimension ref="A3:D45"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <f>A4+1</f>
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f t="shared" ref="A6:A23" si="0">A5+1</f>
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <f t="shared" ref="A24:A29" si="1">A23+1</f>
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <f t="shared" ref="A30:A45" si="2">A29+1</f>
+        <v>27</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0003AC-73A6-714F-9EC1-A32D17819750}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
@@ -3981,645 +5034,6 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7D17F3-EDCF-734A-BF3E-5D3D430502FC}">
-  <dimension ref="A3:D45"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <f>A4+1</f>
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <f t="shared" ref="A6:A23" si="0">A5+1</f>
-        <v>3</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
-        <f t="shared" ref="A24:A29" si="1">A23+1</f>
-        <v>21</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
-        <f t="shared" ref="A30:A45" si="2">A29+1</f>
-        <v>27</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
-        <f t="shared" si="2"/>
-        <v>33</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
-        <f t="shared" si="2"/>
-        <v>37</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
-        <f t="shared" si="2"/>
-        <v>38</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
-        <f t="shared" si="2"/>
-        <v>39</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
-        <f t="shared" si="2"/>
-        <v>41</v>
-      </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
-        <f t="shared" si="2"/>
-        <v>42</v>
-      </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4870,10 +5284,268 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{458EFE0B-2BF2-C048-9F04-D346A5E87B88}">
+  <dimension ref="A2:AG14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT("CREATE TABLE ",CHAR(34),B2,CHAR(34),"(")</f>
+        <v>CREATE TABLE "T_POST_BID"(</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f>Columns!B10</f>
+        <v>ID</v>
+      </c>
+      <c r="C5" s="3" t="str">
+        <f>Columns!C10</f>
+        <v>VARCHAR(50) NOT NULL</v>
+      </c>
+      <c r="D5" s="3" t="str">
+        <f>Columns!D10</f>
+        <v>table id</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xlfn.CONCAT(CHAR(34),B5, CHAR(34)," ",C5, ",")</f>
+        <v>"ID" VARCHAR(50) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <f>A5+1</f>
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <f>Columns!B37</f>
+        <v>POST_ID</v>
+      </c>
+      <c r="C6" s="3" t="str">
+        <f>Columns!C37</f>
+        <v>VARCHAR(50) NOT NULL</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f>Columns!D37</f>
+        <v>Post table id</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" ref="F6:F13" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
+        <v>"POST_ID" VARCHAR(50) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <f t="shared" ref="A7:A14" si="1">A6+1</f>
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="str">
+        <f>Columns!B36</f>
+        <v>REQUEST_USER_ID</v>
+      </c>
+      <c r="C7" s="3" t="str">
+        <f>Columns!C36</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D7" s="3" t="str">
+        <f>Columns!D36</f>
+        <v>User Id</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>"REQUEST_USER_ID" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="str">
+        <f>Columns!B42</f>
+        <v>AMOUNT</v>
+      </c>
+      <c r="C8" s="3" t="str">
+        <f>Columns!C42</f>
+        <v>int NOT NULL</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f>Columns!D42</f>
+        <v>Amount</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>"AMOUNT" int NOT NULL,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f>CommonColumns!B4</f>
+        <v>DEL_FLG</v>
+      </c>
+      <c r="C9" s="3" t="str">
+        <f>CommonColumns!C4</f>
+        <v>int DEFAULT 0</v>
+      </c>
+      <c r="D9" s="3" t="str">
+        <f>CommonColumns!D4</f>
+        <v>delete flag</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>"DEL_FLG" int DEFAULT 0,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="str">
+        <f>CommonColumns!B5</f>
+        <v>INS_DT</v>
+      </c>
+      <c r="C10" s="3" t="str">
+        <f>CommonColumns!C5</f>
+        <v>TIMESTAMP DEFAULT CURRENT_TIMESTAMP</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f>CommonColumns!D5</f>
+        <v>Inserted date</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_DT" TIMESTAMP DEFAULT CURRENT_TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f>CommonColumns!B6</f>
+        <v>INS_BY</v>
+      </c>
+      <c r="C11" s="3" t="str">
+        <f>CommonColumns!C6</f>
+        <v>VARCHAR(250) NOT NULL</v>
+      </c>
+      <c r="D11" s="3" t="str">
+        <f>CommonColumns!D6</f>
+        <v xml:space="preserve">Inserted by </v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>"INS_BY" VARCHAR(250) NOT NULL,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="str">
+        <f>CommonColumns!B7</f>
+        <v>UPD_DT</v>
+      </c>
+      <c r="C12" s="3" t="str">
+        <f>CommonColumns!C7</f>
+        <v>TIMESTAMP</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>CommonColumns!D7</f>
+        <v>Updated date</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>"UPD_DT" TIMESTAMP,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B13" s="3" t="str">
+        <f>CommonColumns!B8</f>
+        <v>UPD_BY</v>
+      </c>
+      <c r="C13" s="3" t="str">
+        <f>CommonColumns!C8</f>
+        <v>VARCHAR(250)</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f>CommonColumns!D8</f>
+        <v>Updated by</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>"UPD_BY" VARCHAR(250),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAD4CD2-793C-F541-AD63-B0A103A94339}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -5129,7 +5801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705A2A03-52BE-704A-B9B0-E08FD94F4E0C}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
@@ -5389,7 +6061,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B493808A-68C4-EA4D-94DE-B822277B2CB8}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
@@ -5649,7 +6321,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9FD591B-EA50-FE4F-A794-48E803E9E6A3}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
@@ -5883,7 +6555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1940831B-3034-354F-A9B0-BA947E4E5A0B}">
   <dimension ref="A2:AG20"/>
   <sheetViews>
@@ -6167,402 +6839,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D308D1A-EFEE-6845-8598-73802D5A6ADD}">
-  <dimension ref="A2:AG21"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="C3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="AG3" s="1"/>
-    </row>
-    <row r="4" spans="1:33" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="str">
-        <f>_xlfn.CONCAT("CREATE TABLE ",CHAR(34),B2,CHAR(34),"(")</f>
-        <v>CREATE TABLE "T_POST"(</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="str">
-        <f>Columns!B10</f>
-        <v>ID</v>
-      </c>
-      <c r="C5" s="3" t="str">
-        <f>Columns!C10</f>
-        <v>VARCHAR(50) NOT NULL</v>
-      </c>
-      <c r="D5" s="3" t="str">
-        <f>Columns!D10</f>
-        <v>table id</v>
-      </c>
-      <c r="F5" t="str">
-        <f>_xlfn.CONCAT(CHAR(34),B5, CHAR(34)," ",C5, ",")</f>
-        <v>"ID" VARCHAR(50) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <f>A5+1</f>
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="str">
-        <f>Columns!B11</f>
-        <v>USER_ID</v>
-      </c>
-      <c r="C6" s="3" t="str">
-        <f>Columns!C11</f>
-        <v>VARCHAR(250) NOT NULL</v>
-      </c>
-      <c r="D6" s="3" t="str">
-        <f>Columns!D11</f>
-        <v>User Id</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" ref="F6:F19" si="0">_xlfn.CONCAT(CHAR(34),B6, CHAR(34)," ",C6, ",")</f>
-        <v>"USER_ID" VARCHAR(250) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <f t="shared" ref="A7:A21" si="1">A6+1</f>
-        <v>3</v>
-      </c>
-      <c r="B7" s="3" t="str">
-        <f>Columns!B31</f>
-        <v>SERVICE_ID</v>
-      </c>
-      <c r="C7" s="3" t="str">
-        <f>Columns!C31</f>
-        <v>VARCHAR(50) NOT NULL</v>
-      </c>
-      <c r="D7" s="3" t="str">
-        <f>Columns!D31</f>
-        <v>M_SERVICE table id</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>"SERVICE_ID" VARCHAR(50) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="str">
-        <f>Columns!B25</f>
-        <v>VEHICLE_ID</v>
-      </c>
-      <c r="C8" s="3" t="str">
-        <f>Columns!C25</f>
-        <v xml:space="preserve">VARCHAR(50) </v>
-      </c>
-      <c r="D8" s="3" t="str">
-        <f>Columns!D25</f>
-        <v>Velicle master table id</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>"VEHICLE_ID" VARCHAR(50) ,</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B9" s="3" t="str">
-        <f>Columns!B32</f>
-        <v>ACTIVITY_DATE_TIME_FROM</v>
-      </c>
-      <c r="C9" s="3" t="str">
-        <f>Columns!C32</f>
-        <v>VARCHAR(25)</v>
-      </c>
-      <c r="D9" s="3" t="str">
-        <f>Columns!D32</f>
-        <v>Activity date time from</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>"ACTIVITY_DATE_TIME_FROM" VARCHAR(25),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="str">
-        <f>Columns!B33</f>
-        <v>ACTIVITY_DATE_TIME_TO</v>
-      </c>
-      <c r="C10" s="3" t="str">
-        <f>Columns!C33</f>
-        <v>VARCHAR(25)</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f>Columns!D33</f>
-        <v>Activity date time to</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>"ACTIVITY_DATE_TIME_TO" VARCHAR(25),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="B11" s="3" t="str">
-        <f>Columns!B34</f>
-        <v>SOURCE</v>
-      </c>
-      <c r="C11" s="3" t="str">
-        <f>Columns!C34</f>
-        <v>VARCHAR(500)</v>
-      </c>
-      <c r="D11" s="3" t="str">
-        <f>Columns!D34</f>
-        <v>Source adderss</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>"SOURCE" VARCHAR(500),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="B12" s="3" t="str">
-        <f>Columns!B35</f>
-        <v>DESTINATION</v>
-      </c>
-      <c r="C12" s="3" t="str">
-        <f>Columns!C35</f>
-        <v>VARCHAR(500)</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f>Columns!D35</f>
-        <v>Destination address</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>"DESTINATION" VARCHAR(500),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="str">
-        <f>Columns!B22</f>
-        <v>OTHER</v>
-      </c>
-      <c r="C13" s="3" t="str">
-        <f>Columns!C22</f>
-        <v>TEXT</v>
-      </c>
-      <c r="D13" s="3" t="str">
-        <f>Columns!D22</f>
-        <v>other details</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>"OTHER" TEXT,</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="str">
-        <f>Columns!B23</f>
-        <v>STATUS</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f>Columns!D23</f>
-        <v>status</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>"STATUS" VARCHAR(50) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B15" s="3" t="str">
-        <f>CommonColumns!B4</f>
-        <v>DEL_FLG</v>
-      </c>
-      <c r="C15" s="3" t="str">
-        <f>CommonColumns!C4</f>
-        <v>int DEFAULT 0</v>
-      </c>
-      <c r="D15" s="3" t="str">
-        <f>CommonColumns!D4</f>
-        <v>delete flag</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>"DEL_FLG" int DEFAULT 0,</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="B16" s="3" t="str">
-        <f>CommonColumns!B5</f>
-        <v>INS_DT</v>
-      </c>
-      <c r="C16" s="3" t="str">
-        <f>CommonColumns!C5</f>
-        <v>TIMESTAMP DEFAULT CURRENT_TIMESTAMP</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f>CommonColumns!D5</f>
-        <v>Inserted date</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>"INS_DT" TIMESTAMP DEFAULT CURRENT_TIMESTAMP,</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="B17" s="3" t="str">
-        <f>CommonColumns!B6</f>
-        <v>INS_BY</v>
-      </c>
-      <c r="C17" s="3" t="str">
-        <f>CommonColumns!C6</f>
-        <v>VARCHAR(250) NOT NULL</v>
-      </c>
-      <c r="D17" s="3" t="str">
-        <f>CommonColumns!D6</f>
-        <v xml:space="preserve">Inserted by </v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>"INS_BY" VARCHAR(250) NOT NULL,</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B18" s="3" t="str">
-        <f>CommonColumns!B7</f>
-        <v>UPD_DT</v>
-      </c>
-      <c r="C18" s="3" t="str">
-        <f>CommonColumns!C7</f>
-        <v>TIMESTAMP</v>
-      </c>
-      <c r="D18" s="3" t="str">
-        <f>CommonColumns!D7</f>
-        <v>Updated date</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>"UPD_DT" TIMESTAMP,</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B19" s="3" t="str">
-        <f>CommonColumns!B8</f>
-        <v>UPD_BY</v>
-      </c>
-      <c r="C19" s="3" t="str">
-        <f>CommonColumns!C8</f>
-        <v>VARCHAR(250)</v>
-      </c>
-      <c r="D19" s="3" t="str">
-        <f>CommonColumns!D8</f>
-        <v>Updated by</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>"UPD_BY" VARCHAR(250),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>